<commit_message>
Chekpoint for Joule submission
</commit_message>
<xml_diff>
--- a/documents/coin_cell_tracker.xlsx
+++ b/documents/coin_cell_tracker.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aweng/Documents/project-formation/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193E105B-B98E-DC48-AD80-D755F9B7064D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B80EA2-0703-7445-9195-704FFEA758EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6800" yWindow="5720" windowWidth="25860" windowHeight="14600" xr2:uid="{3F8F1071-436E-EF4A-BDC1-556BB2A45A51}"/>
+    <workbookView xWindow="9280" yWindow="29160" windowWidth="25860" windowHeight="14600" xr2:uid="{3F8F1071-436E-EF4A-BDC1-556BB2A45A51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>cell</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>theoretical_capacity_mah_g</t>
+  </si>
+  <si>
+    <t>we_diameter_mm</t>
+  </si>
+  <si>
+    <t>cell_capacity_mah_cm2</t>
+  </si>
+  <si>
+    <t>we_area_cm2</t>
   </si>
 </sst>
 </file>
@@ -421,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419E6D93-9FAE-4942-B9D3-B9B0D21FA49F}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -437,7 +446,7 @@
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,8 +465,17 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -468,7 +486,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -488,8 +506,19 @@
         <f>(C3-$C$2)*D3/100*E3</f>
         <v>2.15354</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>14</v>
+      </c>
+      <c r="H3">
+        <f>PI() * ( G3 / 2 / 10 )^2</f>
+        <v>1.5393804002589984</v>
+      </c>
+      <c r="I3">
+        <f>F3/H3</f>
+        <v>1.3989654536576341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -509,8 +538,19 @@
         <f>(C4-$C$2)*D4/100*E4</f>
         <v>1.9899800000000005</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>14</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H13" si="0">PI() * ( G4 / 2 / 10 )^2</f>
+        <v>1.5393804002589984</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I13" si="1">F4/H4</f>
+        <v>1.2927149128735103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -527,11 +567,22 @@
         <v>145</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F4:F13" si="0">(C5-$C$2)*D5/100*E5</f>
+        <f t="shared" ref="F5" si="2">(C5-$C$2)*D5/100*E5</f>
         <v>2.0172400000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1.5393804002589984</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>1.3104233363375308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -542,7 +593,7 @@
         <v>6.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -562,8 +613,19 @@
         <f>(C7-$C$6)*D7/100*E7</f>
         <v>2.9327999999999994</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>14</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>1.5393804002589984</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>1.9051821106118803</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -580,11 +642,22 @@
         <v>120</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F9" si="1">(C8-$C$6)*D8/100*E8</f>
+        <f t="shared" ref="F8:F9" si="3">(C8-$C$6)*D8/100*E8</f>
         <v>2.9553600000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>14</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>1.5393804002589984</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>1.9198373576165875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -601,11 +674,22 @@
         <v>120</v>
       </c>
       <c r="F9">
+        <f t="shared" si="3"/>
+        <v>2.7748800000000005</v>
+      </c>
+      <c r="G9">
+        <v>14</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>1.5393804002589984</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="1"/>
-        <v>2.7748800000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.8025953815789335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -616,7 +700,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -636,8 +720,19 @@
         <f>(C11-$C$10)*D11/100*E11</f>
         <v>4.6648799999999992</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>1.5393804002589984</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>3.030362085430697</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -654,11 +749,22 @@
         <v>372</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:F13" si="2">(C12-$C$10)*D12/100*E12</f>
+        <f t="shared" ref="F12:F13" si="4">(C12-$C$10)*D12/100*E12</f>
         <v>4.4881800000000007</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>14</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>1.5393804002589984</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>2.9155756428007473</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -675,8 +781,19 @@
         <v>372</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.594199999999999</v>
+      </c>
+      <c r="G13">
+        <v>14</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>1.5393804002589984</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>2.9844475083787163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>